<commit_message>
Excel → INSERT SQL の更新、PostgreSQL 用とMySQL用を追加
</commit_message>
<xml_diff>
--- a/makeSQL/sample.xlsx
+++ b/makeSQL/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pyspace\LaboA\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\tempA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D56F47F-1B8D-4566-BD66-0607E7D3EF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB8494C-D722-47D8-AA78-3A950CB6448F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="135" windowWidth="21390" windowHeight="14205" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7290" yWindow="2445" windowWidth="15855" windowHeight="10275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T_USERS" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>UID</t>
     <phoneticPr fontId="1"/>
@@ -76,7 +76,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>null</t>
+    <t>LIMIT_DATE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SP_RATIO</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -84,8 +88,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy/mm/d\ hh:mm:ss"/>
+    <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -138,11 +143,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -495,19 +501,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941CAF08-5717-4104-B3DB-B0CFF2BEB79D}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="2" max="3" width="14.75" customWidth="1"/>
-    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="10.625" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,10 +529,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -537,11 +551,17 @@
       <c r="D2" s="1">
         <v>36</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45635</v>
+      </c>
+      <c r="G2" s="2">
         <v>45047.516516203701</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -554,24 +574,32 @@
       <c r="D3" s="1">
         <v>31</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
+        <v>0.215</v>
+      </c>
+      <c r="F3" s="4">
+        <v>45540</v>
+      </c>
+      <c r="G3" s="2">
         <v>45048.516516145835</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45611</v>
+      </c>
+      <c r="G4" s="2">
         <v>45048.516516145835</v>
       </c>
     </row>

</xml_diff>